<commit_message>
termine propuesta de madera
</commit_message>
<xml_diff>
--- a/Proyectos/00-000_EMPRESA_Casa Madera/01_Hojas de calculo/DP - Analisis de cargas.xlsx
+++ b/Proyectos/00-000_EMPRESA_Casa Madera/01_Hojas de calculo/DP - Analisis de cargas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andres\Sigma\Proyectos\00-000_EMPRESA_Casa Madera\01_Hojas de calculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EFB747-DAD6-439D-936F-B067731E66F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163D5E56-0228-409E-95D6-FE4A91AEB229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{5EF5C615-0969-4B44-9BD4-17AD9F6ECA56}"/>
   </bookViews>
@@ -614,6 +614,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,52 +651,48 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,7 +1023,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="63" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1040,7 +1040,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
@@ -1062,13 +1062,13 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="67"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="69"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1119,12 +1119,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="8">
         <f>SUM(E7:E9)</f>
         <v>28.5</v>
@@ -1140,9 +1140,9 @@
       <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="8">
         <v>51</v>
       </c>
@@ -1151,9 +1151,9 @@
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="17">
         <v>-74</v>
       </c>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,27 +1290,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="H1" s="75" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="H1" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="N1" s="75" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="N1" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
@@ -1327,13 +1327,13 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -1357,20 +1357,20 @@
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="76" t="s">
+      <c r="H5" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="N5" s="77" t="s">
@@ -1400,7 +1400,7 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="54" t="s">
@@ -1409,22 +1409,22 @@
       <c r="C7" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="81" t="s">
+      <c r="I7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="81"/>
+      <c r="J7" s="75"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="85" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="54" t="s">
@@ -1438,7 +1438,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="80"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="73"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="29" t="s">
         <v>28</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="N8" s="73"/>
+      <c r="N8" s="86"/>
       <c r="O8" s="29" t="s">
         <v>23</v>
       </c>
@@ -1492,20 +1492,20 @@
       <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="74" t="s">
+      <c r="H10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="N10" s="47" t="s">
@@ -1572,11 +1572,11 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="N12" s="77" t="s">
@@ -1591,8 +1591,7 @@
         <v>67</v>
       </c>
       <c r="B13" s="6">
-        <f>0.03/0.4</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C13" s="6">
         <v>1.6</v>
@@ -1600,7 +1599,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="6">
         <f>+B13*C13</f>
-        <v>0.12</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
@@ -1609,10 +1608,10 @@
       <c r="J13" s="56"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1643,24 +1642,24 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="33">
         <f>SUM(E11:E14)</f>
-        <v>0.8600000000000001</v>
+        <v>0.82000000000000017</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="N15" s="83" t="s">
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="N15" s="81" t="s">
         <v>32</v>
       </c>
       <c r="O15" s="53" t="s">
@@ -1684,7 +1683,7 @@
       <c r="J16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="84"/>
+      <c r="N16" s="82"/>
       <c r="O16" s="29" t="s">
         <v>24</v>
       </c>
@@ -1693,10 +1692,10 @@
       <c r="A17" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="87">
+      <c r="B17" s="62">
         <v>2</v>
       </c>
-      <c r="C17" s="87">
+      <c r="C17" s="62">
         <v>1.6</v>
       </c>
       <c r="D17" s="25" t="s">
@@ -1723,8 +1722,8 @@
       <c r="A18" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="33">
         <v>1</v>
       </c>
@@ -1743,8 +1742,8 @@
       <c r="A19" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="25" t="s">
         <v>12</v>
       </c>
@@ -1766,25 +1765,25 @@
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="85" t="s">
+      <c r="H20" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="81" t="s">
+      <c r="I20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="81"/>
+      <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="85"/>
+      <c r="H21" s="84"/>
       <c r="I21" s="29" t="s">
         <v>28</v>
       </c>
@@ -1812,23 +1811,23 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="81" t="s">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="81"/>
+      <c r="E23" s="75"/>
       <c r="H23" s="45" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
       <c r="D24" s="29" t="s">
         <v>28</v>
       </c>
@@ -1837,56 +1836,56 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="26">
         <f>1.2*$E$15+1.6*$E$17</f>
-        <v>6.152000000000001</v>
+        <v>6.104000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="26">
         <f>1.6*$D$18</f>
         <v>1.6</v>
       </c>
       <c r="E26" s="26">
         <f>1.2*$E$15</f>
-        <v>1.032</v>
+        <v>0.98400000000000021</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
       <c r="D27" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="26">
         <f>1.2*$E$15+1.6*$E$19</f>
-        <v>0.10240000000000005</v>
+        <v>5.4400000000000226E-2</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="76" t="s">
+      <c r="A29" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
@@ -1896,20 +1895,20 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="81" t="s">
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="81"/>
+      <c r="E31" s="75"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
+      <c r="A32" s="74"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="29" t="s">
         <v>28</v>
       </c>
@@ -1918,55 +1917,65 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
       <c r="D33" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="26">
         <f>$E$15+$E$17</f>
-        <v>4.0600000000000005</v>
+        <v>4.0200000000000005</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="82"/>
-      <c r="C34" s="82"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
       <c r="D34" s="26">
         <f>$D$18</f>
         <v>1</v>
       </c>
       <c r="E34" s="26">
         <f>$E$15</f>
-        <v>0.8600000000000001</v>
+        <v>0.82000000000000017</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="82" t="s">
+      <c r="A35" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="82"/>
-      <c r="C35" s="82"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
       <c r="D35" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="26">
         <f>$E$15+$E$19</f>
-        <v>0.27900000000000014</v>
+        <v>0.23900000000000021</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A31:C32"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="H12:J12"/>
     <mergeCell ref="N12:Q12"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="H15:J15"/>
@@ -1983,21 +1992,11 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A31:C32"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2029,27 +2028,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="H1" s="75" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="H1" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="N1" s="75" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="N1" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
@@ -2066,13 +2065,13 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -2096,20 +2095,20 @@
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="76" t="s">
+      <c r="H5" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="N5" s="77" t="s">
@@ -2139,7 +2138,7 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -2148,22 +2147,22 @@
       <c r="C7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="81" t="s">
+      <c r="I7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="81"/>
+      <c r="J7" s="75"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="85" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="43" t="s">
@@ -2177,7 +2176,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="80"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2191,7 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="73"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="29" t="s">
         <v>28</v>
       </c>
@@ -2201,7 +2200,7 @@
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="N8" s="73"/>
+      <c r="N8" s="86"/>
       <c r="O8" s="29" t="s">
         <v>23</v>
       </c>
@@ -2231,20 +2230,20 @@
       <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="74" t="s">
+      <c r="H10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="N10" s="47" t="s">
@@ -2311,11 +2310,11 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="N12" s="77" t="s">
@@ -2354,24 +2353,24 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
       <c r="E14" s="33">
         <f>SUM(E11:E13)</f>
         <v>0.245</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="74" t="s">
+      <c r="H14" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="N14" s="83" t="s">
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="N14" s="81" t="s">
         <v>32</v>
       </c>
       <c r="O14" s="36" t="s">
@@ -2395,7 +2394,7 @@
       <c r="J15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="84"/>
+      <c r="N15" s="82"/>
       <c r="O15" s="29" t="s">
         <v>24</v>
       </c>
@@ -2404,8 +2403,8 @@
       <c r="A16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="25" t="s">
         <v>12</v>
       </c>
@@ -2429,8 +2428,8 @@
       <c r="A17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="33">
         <v>1</v>
       </c>
@@ -2449,8 +2448,8 @@
       <c r="A18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="25" t="s">
         <v>12</v>
       </c>
@@ -2472,25 +2471,25 @@
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="85" t="s">
+      <c r="H19" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="81" t="s">
+      <c r="I19" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="81"/>
+      <c r="J19" s="75"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="85"/>
+      <c r="H20" s="84"/>
       <c r="I20" s="29" t="s">
         <v>28</v>
       </c>
@@ -2518,7 +2517,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="85" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="55" t="s">
@@ -2538,7 +2537,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="29" t="s">
         <v>24</v>
       </c>
@@ -2625,13 +2624,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
@@ -2641,20 +2640,20 @@
       <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="81" t="s">
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="81"/>
+      <c r="E30" s="75"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
+      <c r="A31" s="74"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="29" t="s">
         <v>28</v>
       </c>
@@ -2663,11 +2662,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
       <c r="D32" s="16" t="s">
         <v>12</v>
       </c>
@@ -2677,11 +2676,11 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
       <c r="D33" s="26">
         <f>$D$17</f>
         <v>1</v>
@@ -2692,11 +2691,11 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="82"/>
-      <c r="C34" s="82"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
       <c r="D34" s="16" t="s">
         <v>12</v>
       </c>
@@ -2707,11 +2706,26 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="H19:H20"/>
@@ -2720,26 +2734,11 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>